<commit_message>
SQL HISTORY STATEMENTS FIXED
</commit_message>
<xml_diff>
--- a/reports/2022.01.18 tas-diff-add-del.xlsx
+++ b/reports/2022.01.18 tas-diff-add-del.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dompa\Documents\GitHub\tas-diff-add-del\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmpannone\Documents\GitHub\tas-diff-add-del\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7669CEFB-ED12-4F3B-9AA0-B46C6CE9B5E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{54179605-623F-451C-80A0-178266E58FA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8724"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8772"/>
   </bookViews>
   <sheets>
     <sheet name="2022.01.18 tas-diff-add-del" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="237">
   <si>
     <t>REGION</t>
   </si>
@@ -239,9 +239,6 @@
   </si>
   <si>
     <t>ADDED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1) 2022.01.18 (DELETED) </t>
   </si>
   <si>
     <t>CR22 Mat-Su District NHS Preventative Maintenance CFHWY00861 / 0001733
@@ -381,9 +378,6 @@
   </si>
   <si>
     <t>Marine Highways</t>
-  </si>
-  <si>
-    <t>(1) 2022.01.18 ANTADVDT December 2022</t>
   </si>
   <si>
     <t>AUKE BAY TERMINAL BUILDING AND ELECTRICAL IMPROVEMENTS</t>
@@ -618,9 +612,6 @@
     <t>Between $500,000 and $1,000,000</t>
   </si>
   <si>
-    <t xml:space="preserve">(1) 2022.01.18 DESCRIPTION </t>
-  </si>
-  <si>
     <t>HNS MOSQUITO LAKE ROAD #550474 - DEC 20 SE PR</t>
   </si>
   <si>
@@ -684,9 +675,6 @@
   </si>
   <si>
     <t>Reconstruct the Haines Highway from milepost 20.0 to 25.0 including the Chilkat River Bridge is the next and final phase to advertise</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1) 2022.01.18 ADDLINFO </t>
   </si>
   <si>
     <t>KDK: ADQ AIRPORT APRON AND TWY C, D AND F REHAB</t>
@@ -1670,8 +1658,8 @@
     <col min="6" max="6" width="65.77734375" customWidth="1"/>
     <col min="7" max="7" width="23.77734375" style="9" customWidth="1"/>
     <col min="8" max="8" width="10.77734375" customWidth="1"/>
-    <col min="9" max="12" width="15.77734375" customWidth="1"/>
-    <col min="13" max="13" width="100.77734375" customWidth="1"/>
+    <col min="9" max="13" width="15.77734375" customWidth="1"/>
+    <col min="14" max="14" width="100.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="3" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2079,38 +2067,35 @@
       <c r="B11" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="G11" s="9" t="s">
         <v>74</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>75</v>
       </c>
       <c r="H11" s="1">
         <v>44562</v>
       </c>
       <c r="I11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K11" t="s">
         <v>42</v>
       </c>
       <c r="L11" t="s">
+        <v>76</v>
+      </c>
+      <c r="M11" t="s">
         <v>77</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>78</v>
       </c>
-      <c r="N11" t="s">
+      <c r="P11" t="s">
         <v>79</v>
-      </c>
-      <c r="P11" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2121,7 +2106,7 @@
         <v>72</v>
       </c>
       <c r="F12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>34</v>
@@ -2130,22 +2115,22 @@
         <v>44652</v>
       </c>
       <c r="I12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K12" t="s">
         <v>42</v>
       </c>
       <c r="L12" t="s">
+        <v>82</v>
+      </c>
+      <c r="M12" t="s">
         <v>83</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>84</v>
-      </c>
-      <c r="N12" t="s">
-        <v>85</v>
       </c>
       <c r="P12" t="s">
         <v>32</v>
@@ -2165,7 +2150,7 @@
         <v>44593</v>
       </c>
       <c r="F13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G13" s="9" t="s">
         <v>34</v>
@@ -2174,7 +2159,7 @@
         <v>44593</v>
       </c>
       <c r="I13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2191,7 +2176,7 @@
         <v>44621</v>
       </c>
       <c r="F14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G14" s="9" t="s">
         <v>34</v>
@@ -2200,7 +2185,7 @@
         <v>44621</v>
       </c>
       <c r="I14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2217,16 +2202,16 @@
         <v>44593</v>
       </c>
       <c r="F15" t="s">
+        <v>89</v>
+      </c>
+      <c r="G15" s="9" t="s">
         <v>90</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>91</v>
       </c>
       <c r="H15" s="1">
         <v>44593</v>
       </c>
       <c r="I15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2243,7 +2228,7 @@
         <v>44621</v>
       </c>
       <c r="F16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G16" s="9" t="s">
         <v>55</v>
@@ -2252,7 +2237,7 @@
         <v>44621</v>
       </c>
       <c r="I16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2269,7 +2254,7 @@
         <v>44652</v>
       </c>
       <c r="F17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G17" s="9" t="s">
         <v>34</v>
@@ -2278,7 +2263,7 @@
         <v>44652</v>
       </c>
       <c r="I17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2295,16 +2280,16 @@
         <v>44652</v>
       </c>
       <c r="F18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G18" s="9" t="s">
         <v>97</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>98</v>
       </c>
       <c r="H18" s="1">
         <v>44652</v>
       </c>
       <c r="I18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2321,16 +2306,16 @@
         <v>44682</v>
       </c>
       <c r="F19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H19" s="1">
         <v>44682</v>
       </c>
       <c r="I19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2347,7 +2332,7 @@
         <v>44743</v>
       </c>
       <c r="F20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G20" s="9" t="s">
         <v>34</v>
@@ -2356,7 +2341,7 @@
         <v>44743</v>
       </c>
       <c r="I20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2373,7 +2358,7 @@
         <v>44682</v>
       </c>
       <c r="F21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G21" s="9" t="s">
         <v>34</v>
@@ -2382,7 +2367,7 @@
         <v>44682</v>
       </c>
       <c r="I21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2399,7 +2384,7 @@
         <v>44682</v>
       </c>
       <c r="F22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G22" s="9" t="s">
         <v>34</v>
@@ -2408,7 +2393,7 @@
         <v>44682</v>
       </c>
       <c r="I22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2425,16 +2410,16 @@
         <v>44896</v>
       </c>
       <c r="F23" t="s">
+        <v>107</v>
+      </c>
+      <c r="G23" s="9" t="s">
         <v>108</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>109</v>
       </c>
       <c r="H23" s="1">
         <v>44896</v>
       </c>
       <c r="I23" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2451,7 +2436,7 @@
         <v>44621</v>
       </c>
       <c r="F24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G24" s="9" t="s">
         <v>19</v>
@@ -2460,7 +2445,7 @@
         <v>44621</v>
       </c>
       <c r="I24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2471,22 +2456,22 @@
         <v>13</v>
       </c>
       <c r="C25" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="D25" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="D25" s="9" t="s">
-        <v>114</v>
-      </c>
       <c r="F25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H25" s="1">
         <v>44682</v>
       </c>
       <c r="I25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2497,22 +2482,22 @@
         <v>12</v>
       </c>
       <c r="C26" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D26" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="D26" s="9" t="s">
-        <v>116</v>
-      </c>
       <c r="F26" t="s">
+        <v>89</v>
+      </c>
+      <c r="G26" s="9" t="s">
         <v>90</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>91</v>
       </c>
       <c r="H26" s="1">
         <v>44593</v>
       </c>
       <c r="I26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2523,60 +2508,57 @@
         <v>12</v>
       </c>
       <c r="C27" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D27" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="F27" t="s">
         <v>116</v>
       </c>
-      <c r="F27" t="s">
-        <v>117</v>
-      </c>
       <c r="G27" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H27" s="1">
         <v>44682</v>
       </c>
       <c r="I27" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
+        <v>119</v>
+      </c>
+      <c r="G28" s="9" t="s">
         <v>120</v>
-      </c>
-      <c r="F28" t="s">
-        <v>121</v>
-      </c>
-      <c r="G28" s="9" t="s">
-        <v>122</v>
       </c>
       <c r="H28" s="1">
         <v>44896</v>
       </c>
       <c r="I28" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J28" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="K28">
         <v>9500150</v>
       </c>
       <c r="L28" t="s">
+        <v>122</v>
+      </c>
+      <c r="M28" t="s">
+        <v>123</v>
+      </c>
+      <c r="N28" t="s">
         <v>124</v>
-      </c>
-      <c r="M28" t="s">
-        <v>125</v>
-      </c>
-      <c r="N28" t="s">
-        <v>126</v>
       </c>
       <c r="P28" t="s">
         <v>39</v>
@@ -2584,119 +2566,119 @@
     </row>
     <row r="29" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>72</v>
       </c>
       <c r="F29" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H29" s="1">
         <v>44621</v>
       </c>
       <c r="I29" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="J29" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="K29">
         <v>652016</v>
       </c>
       <c r="L29" t="s">
+        <v>129</v>
+      </c>
+      <c r="M29" t="s">
+        <v>130</v>
+      </c>
+      <c r="N29" t="s">
         <v>131</v>
       </c>
-      <c r="M29" t="s">
+      <c r="O29" t="s">
         <v>132</v>
       </c>
-      <c r="N29" t="s">
+      <c r="P29" t="s">
         <v>133</v>
-      </c>
-      <c r="O29" t="s">
-        <v>134</v>
-      </c>
-      <c r="P29" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>72</v>
       </c>
       <c r="F30" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H30" s="1">
         <v>44896</v>
       </c>
       <c r="I30" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J30" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="K30">
         <v>713010</v>
       </c>
       <c r="L30" t="s">
+        <v>136</v>
+      </c>
+      <c r="M30" t="s">
+        <v>137</v>
+      </c>
+      <c r="N30" t="s">
         <v>138</v>
       </c>
-      <c r="M30" t="s">
+      <c r="O30" t="s">
         <v>139</v>
       </c>
-      <c r="N30" t="s">
+      <c r="P30" t="s">
         <v>140</v>
-      </c>
-      <c r="O30" t="s">
-        <v>141</v>
-      </c>
-      <c r="P30" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>72</v>
       </c>
       <c r="F31" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H31" s="1">
         <v>44896</v>
       </c>
       <c r="I31" t="s">
+        <v>143</v>
+      </c>
+      <c r="J31" t="s">
+        <v>143</v>
+      </c>
+      <c r="K31" t="s">
+        <v>144</v>
+      </c>
+      <c r="L31" t="s">
+        <v>129</v>
+      </c>
+      <c r="M31" t="s">
+        <v>130</v>
+      </c>
+      <c r="N31" t="s">
         <v>145</v>
-      </c>
-      <c r="J31" t="s">
-        <v>145</v>
-      </c>
-      <c r="K31" t="s">
-        <v>146</v>
-      </c>
-      <c r="L31" t="s">
-        <v>131</v>
-      </c>
-      <c r="M31" t="s">
-        <v>132</v>
-      </c>
-      <c r="N31" t="s">
-        <v>147</v>
       </c>
       <c r="P31" t="s">
         <v>63</v>
@@ -2704,33 +2686,33 @@
     </row>
     <row r="32" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C32" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="F32" t="s">
         <v>148</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="G32" s="9" t="s">
         <v>149</v>
-      </c>
-      <c r="F32" t="s">
-        <v>150</v>
-      </c>
-      <c r="G32" s="9" t="s">
-        <v>151</v>
       </c>
       <c r="H32" s="1">
         <v>44593</v>
       </c>
       <c r="I32" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="33" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>7</v>
@@ -2742,21 +2724,21 @@
         <v>44621</v>
       </c>
       <c r="F33" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H33" s="1">
         <v>44621</v>
       </c>
       <c r="I33" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>7</v>
@@ -2768,21 +2750,21 @@
         <v>44593</v>
       </c>
       <c r="F34" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H34" s="1">
         <v>44593</v>
       </c>
       <c r="I34" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="35" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>7</v>
@@ -2794,21 +2776,21 @@
         <v>44621</v>
       </c>
       <c r="F35" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G35" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H35" s="1">
         <v>44621</v>
       </c>
       <c r="I35" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="36" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>7</v>
@@ -2820,21 +2802,21 @@
         <v>44621</v>
       </c>
       <c r="F36" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H36" s="1">
         <v>44621</v>
       </c>
       <c r="I36" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>7</v>
@@ -2846,73 +2828,73 @@
         <v>44621</v>
       </c>
       <c r="F37" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G37" s="9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H37" s="1">
         <v>44621</v>
       </c>
       <c r="I37" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="38" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C38" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="F38" t="s">
         <v>167</v>
       </c>
-      <c r="D38" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="F38" t="s">
-        <v>169</v>
-      </c>
       <c r="G38" s="9" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H38" s="1">
         <v>44621</v>
       </c>
       <c r="I38" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C39" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="F39" t="s">
         <v>171</v>
       </c>
-      <c r="D39" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="F39" t="s">
-        <v>173</v>
-      </c>
       <c r="G39" s="9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H39" s="1">
         <v>44621</v>
       </c>
       <c r="I39" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>15</v>
@@ -2921,21 +2903,21 @@
         <v>39</v>
       </c>
       <c r="F40" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G40" s="9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H40" s="1">
         <v>44593</v>
       </c>
       <c r="I40" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="41" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>10</v>
@@ -2944,24 +2926,24 @@
         <v>42</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F41" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G41" s="9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H41" s="1">
         <v>44593</v>
       </c>
       <c r="I41" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="42" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>10</v>
@@ -2970,24 +2952,24 @@
         <v>42</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F42" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G42" s="9" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H42" s="1">
         <v>44621</v>
       </c>
       <c r="I42" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="43" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>10</v>
@@ -2996,24 +2978,24 @@
         <v>42</v>
       </c>
       <c r="D43" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="F43" t="s">
+        <v>174</v>
+      </c>
+      <c r="G43" s="9" t="s">
         <v>175</v>
-      </c>
-      <c r="F43" t="s">
-        <v>176</v>
-      </c>
-      <c r="G43" s="9" t="s">
-        <v>177</v>
       </c>
       <c r="H43" s="1">
         <v>44621</v>
       </c>
       <c r="I43" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="44" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>10</v>
@@ -3022,132 +3004,132 @@
         <v>42</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F44" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G44" s="9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H44" s="1">
         <v>44621</v>
       </c>
       <c r="I44" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="45" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B45" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F45" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G45" s="9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H45" s="1">
         <v>44621</v>
       </c>
       <c r="I45" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="46" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F46" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H46" s="1">
         <v>44593</v>
       </c>
       <c r="I46" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="47" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F47" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G47" s="9" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H47" s="1">
         <v>44621</v>
       </c>
       <c r="I47" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="48" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>17</v>
       </c>
       <c r="F48" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G48" s="9" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="H48" s="1">
         <v>44531</v>
       </c>
       <c r="I48" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="J48" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="K48">
         <v>933042</v>
       </c>
       <c r="L48" t="s">
+        <v>183</v>
+      </c>
+      <c r="M48" t="s">
+        <v>184</v>
+      </c>
+      <c r="N48" t="s">
         <v>185</v>
-      </c>
-      <c r="M48" t="s">
-        <v>186</v>
-      </c>
-      <c r="N48" t="s">
-        <v>187</v>
       </c>
       <c r="P48" t="s">
         <v>25</v>
@@ -3155,154 +3137,151 @@
     </row>
     <row r="49" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>72</v>
       </c>
       <c r="F49" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G49" s="9" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H49" s="1">
         <v>44562</v>
       </c>
       <c r="I49" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="J49" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="K49" t="s">
         <v>42</v>
       </c>
       <c r="L49" t="s">
+        <v>188</v>
+      </c>
+      <c r="M49" t="s">
+        <v>189</v>
+      </c>
+      <c r="N49" t="s">
         <v>190</v>
       </c>
-      <c r="M49" t="s">
+      <c r="P49" t="s">
         <v>191</v>
-      </c>
-      <c r="N49" t="s">
-        <v>192</v>
-      </c>
-      <c r="P49" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="50" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E50" t="s">
-        <v>194</v>
-      </c>
       <c r="F50" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G50" s="9" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="H50" s="1">
         <v>44621</v>
       </c>
       <c r="I50" t="s">
+        <v>194</v>
+      </c>
+      <c r="J50" t="s">
+        <v>194</v>
+      </c>
+      <c r="K50" t="s">
+        <v>195</v>
+      </c>
+      <c r="L50" t="s">
+        <v>196</v>
+      </c>
+      <c r="M50" t="s">
         <v>197</v>
       </c>
-      <c r="J50" t="s">
-        <v>197</v>
-      </c>
-      <c r="K50" t="s">
+      <c r="N50" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="L50" t="s">
-        <v>199</v>
-      </c>
-      <c r="M50" t="s">
-        <v>200</v>
-      </c>
-      <c r="N50" s="2" t="s">
-        <v>201</v>
-      </c>
       <c r="P50" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="51" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>72</v>
       </c>
       <c r="F51" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="G51" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H51" s="1">
         <v>44652</v>
       </c>
       <c r="I51" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="J51" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="K51" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="L51" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="M51" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="N51" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="P51" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="52" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>72</v>
       </c>
       <c r="F52" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="G52" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H52" s="1">
         <v>44896</v>
       </c>
       <c r="I52" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="J52" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="K52">
         <v>9500155</v>
       </c>
       <c r="L52" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M52" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N52" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="P52" t="s">
         <v>25</v>
@@ -3310,40 +3289,40 @@
     </row>
     <row r="53" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>72</v>
       </c>
       <c r="F53" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="G53" s="9" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="H53" s="1">
         <v>44896</v>
       </c>
       <c r="I53" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="J53" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="K53">
         <v>956028</v>
       </c>
       <c r="L53" t="s">
+        <v>208</v>
+      </c>
+      <c r="M53" t="s">
+        <v>209</v>
+      </c>
+      <c r="N53" t="s">
+        <v>210</v>
+      </c>
+      <c r="O53" t="s">
         <v>211</v>
-      </c>
-      <c r="M53" t="s">
-        <v>212</v>
-      </c>
-      <c r="N53" t="s">
-        <v>213</v>
-      </c>
-      <c r="O53" t="s">
-        <v>214</v>
       </c>
       <c r="P53" t="s">
         <v>63</v>
@@ -3351,40 +3330,37 @@
     </row>
     <row r="54" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E54" t="s">
-        <v>215</v>
-      </c>
       <c r="F54" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="G54" s="9" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="H54" s="1">
         <v>44896</v>
       </c>
       <c r="I54" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="J54" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="K54" t="s">
         <v>42</v>
       </c>
       <c r="L54" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="M54" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="N54" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="P54" t="s">
         <v>63</v>
@@ -3392,75 +3368,75 @@
     </row>
     <row r="55" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>72</v>
       </c>
       <c r="F55" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="G55" s="9" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="H55" s="1">
         <v>44896</v>
       </c>
       <c r="I55" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="J55" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="K55" t="s">
         <v>42</v>
       </c>
       <c r="L55" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="M55" t="s">
+        <v>216</v>
+      </c>
+      <c r="N55" t="s">
         <v>220</v>
-      </c>
-      <c r="N55" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="56" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>72</v>
       </c>
       <c r="F56" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="G56" s="9" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="H56" s="1">
         <v>44896</v>
       </c>
       <c r="I56" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="J56" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K56" t="s">
         <v>42</v>
       </c>
       <c r="L56" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="M56" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="N56" s="2" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="O56" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="P56" t="s">
         <v>25</v>
@@ -3468,7 +3444,7 @@
     </row>
     <row r="57" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B57" s="6" t="s">
         <v>7</v>
@@ -3480,91 +3456,91 @@
         <v>44743</v>
       </c>
       <c r="F57" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="G57" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H57" s="1">
         <v>44743</v>
       </c>
       <c r="I57" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="58" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B58" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="F58" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="G58" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H58" s="1">
         <v>44562</v>
       </c>
       <c r="I58" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="59" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B59" s="7" t="s">
         <v>15</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F59" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="G59" s="9" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="H59" s="1">
         <v>44713</v>
       </c>
       <c r="I59" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="60" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B60" s="7" t="s">
         <v>15</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F60" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="G60" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H60" s="1">
         <v>44835</v>
       </c>
       <c r="I60" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>

</xml_diff>